<commit_message>
Minor changes in exercises 1 to 3
</commit_message>
<xml_diff>
--- a/MobileDevOps-PartnerTraining-Outline.xlsx
+++ b/MobileDevOps-PartnerTraining-Outline.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="69">
   <si>
     <t>Welcome, introduction, organizational matters, brief overview of the workshop</t>
   </si>
@@ -43,18 +43,6 @@
   </si>
   <si>
     <t>Motivation of Microsoft to not just continue the way of the past with .NET (importance of cross-platform, modern architecture, open-source, etc.)</t>
-  </si>
-  <si>
-    <t>Describe that we now focus on the production version of .NET (4.6), ASP.NET Core Preview follows later.</t>
-  </si>
-  <si>
-    <t>NuGet as a delivery mechanism for .NET components</t>
-  </si>
-  <si>
-    <t>Growing importance of NuGet for Microsoft-oriented development teams</t>
-  </si>
-  <si>
-    <t>nuget.org vs. private feeds in the cloud (e.g. myget) vs. private feeds on-premise</t>
   </si>
   <si>
     <t>(Option if you have some Devs in the audience) Debug the application to give attendees a deeper insight into the structure of the application</t>
@@ -256,9 +244,6 @@
   </si>
   <si>
     <t>Discuss the need of (external) services in mobile scenarios</t>
-  </si>
-  <si>
-    <t>Show push notifications using Azure Mobile Apps</t>
   </si>
   <si>
     <t>Describe the impact of services for DevOps</t>
@@ -422,7 +407,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -491,24 +476,13 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -625,9 +599,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="15" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -637,6 +608,9 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="5" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -654,9 +628,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="8" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1038,11 +1009,11 @@
     <outlinePr summaryBelow="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:D78"/>
+  <dimension ref="A1:D73"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C28" sqref="C28"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
@@ -1056,16 +1027,16 @@
     <row r="1" spans="1:4" ht="155.1" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="22" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B3" s="23" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="C3" s="24" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D3" s="25" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
@@ -1097,7 +1068,7 @@
         <v>1</v>
       </c>
       <c r="B6" s="46" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="C6" s="46"/>
       <c r="D6" s="27">
@@ -1107,7 +1078,7 @@
     <row r="7" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20"/>
       <c r="B7" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C7" s="35" t="s">
         <v>3</v>
@@ -1117,7 +1088,7 @@
     <row r="8" spans="1:4" s="21" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A8" s="20"/>
       <c r="B8" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C8" s="35" t="s">
         <v>4</v>
@@ -1127,241 +1098,241 @@
     <row r="9" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A9" s="20"/>
       <c r="B9" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C9" s="35" t="s">
-        <v>5</v>
+        <v>33</v>
       </c>
       <c r="D9" s="36"/>
     </row>
     <row r="10" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A10" s="20"/>
       <c r="B10" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C10" s="35" t="s">
-        <v>6</v>
+        <v>34</v>
       </c>
       <c r="D10" s="36"/>
     </row>
     <row r="11" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A11" s="20"/>
       <c r="B11" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C11" s="35" t="s">
-        <v>7</v>
+        <v>32</v>
       </c>
       <c r="D11" s="36"/>
     </row>
     <row r="12" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A12" s="20"/>
       <c r="B12" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C12" s="35" t="s">
-        <v>8</v>
+        <v>36</v>
       </c>
       <c r="D12" s="36"/>
     </row>
     <row r="13" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A13" s="20"/>
       <c r="B13" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C13" s="35" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D13" s="36"/>
     </row>
     <row r="14" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A14" s="20"/>
       <c r="B14" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C14" s="35" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D14" s="36"/>
     </row>
     <row r="15" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A15" s="20"/>
       <c r="B15" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C15" s="35" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="D15" s="36"/>
     </row>
-    <row r="16" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="20"/>
-      <c r="B16" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="35" t="s">
+    <row r="16" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16" s="26">
+        <v>2</v>
+      </c>
+      <c r="B16" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="D16" s="36"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="27">
+        <v>75</v>
+      </c>
     </row>
     <row r="17" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A17" s="20"/>
       <c r="B17" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C17" s="35" t="s">
-        <v>39</v>
+        <v>61</v>
       </c>
       <c r="D17" s="36"/>
     </row>
-    <row r="18" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="20"/>
+    <row r="18" spans="1:4" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="12"/>
       <c r="B18" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C18" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C18" s="37" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="36"/>
-    </row>
-    <row r="19" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="20"/>
+      <c r="D18" s="38"/>
+    </row>
+    <row r="19" spans="1:4" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="12"/>
       <c r="B19" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C19" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="C19" s="37" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="36"/>
-    </row>
-    <row r="20" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="26">
-        <v>2</v>
-      </c>
-      <c r="B20" s="46" t="s">
-        <v>44</v>
-      </c>
-      <c r="C20" s="46"/>
-      <c r="D20" s="27">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="20"/>
+      <c r="D19" s="38"/>
+    </row>
+    <row r="20" spans="1:4" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="12"/>
+      <c r="B20" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="D20" s="38"/>
+    </row>
+    <row r="21" spans="1:4" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="12"/>
       <c r="B21" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C21" s="35" t="s">
-        <v>65</v>
-      </c>
-      <c r="D21" s="36"/>
+        <v>26</v>
+      </c>
+      <c r="C21" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="38"/>
     </row>
     <row r="22" spans="1:4" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A22" s="12"/>
       <c r="B22" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="D22" s="38"/>
+    </row>
+    <row r="23" spans="1:4" s="21" customFormat="1" ht="43.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="20"/>
+      <c r="B23" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="35" t="s">
+        <v>68</v>
+      </c>
+      <c r="D23" s="36"/>
+    </row>
+    <row r="24" spans="1:4" s="21" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="20"/>
+      <c r="B24" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="D24" s="36"/>
+    </row>
+    <row r="25" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="12"/>
+      <c r="B25" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C25" s="48"/>
+      <c r="D25" s="18">
         <v>30</v>
       </c>
-      <c r="C22" s="37" t="s">
-        <v>45</v>
-      </c>
-      <c r="D22" s="38"/>
-    </row>
-    <row r="23" spans="1:4" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="12"/>
-      <c r="B23" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C23" s="37" t="s">
-        <v>46</v>
-      </c>
-      <c r="D23" s="38"/>
-    </row>
-    <row r="24" spans="1:4" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="12"/>
-      <c r="B24" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>50</v>
-      </c>
-      <c r="D24" s="38"/>
-    </row>
-    <row r="25" spans="1:4" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="12"/>
-      <c r="B25" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C25" s="37" t="s">
-        <v>47</v>
-      </c>
-      <c r="D25" s="38"/>
-    </row>
-    <row r="26" spans="1:4" s="10" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="12"/>
-      <c r="B26" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="37" t="s">
-        <v>48</v>
-      </c>
-      <c r="D26" s="38"/>
-    </row>
-    <row r="27" spans="1:4" s="21" customFormat="1" ht="43.5" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="26" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A26" s="26">
+        <v>3</v>
+      </c>
+      <c r="B26" s="46" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" s="46"/>
+      <c r="D26" s="27">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" s="21" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A27" s="20"/>
       <c r="B27" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C27" s="35" t="s">
-        <v>73</v>
+        <v>27</v>
       </c>
       <c r="D27" s="36"/>
     </row>
-    <row r="28" spans="1:4" s="21" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A28" s="20"/>
       <c r="B28" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C28" s="35" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="D28" s="36"/>
     </row>
-    <row r="29" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="12"/>
-      <c r="B29" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C29" s="48"/>
-      <c r="D29" s="18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A30" s="26">
-        <v>3</v>
-      </c>
-      <c r="B30" s="46" t="s">
-        <v>2</v>
-      </c>
-      <c r="C30" s="46"/>
-      <c r="D30" s="27">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" s="21" customFormat="1" ht="30" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="20"/>
+      <c r="B29" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C29" s="35" t="s">
+        <v>13</v>
+      </c>
+      <c r="D29" s="36"/>
+    </row>
+    <row r="30" spans="1:4" s="21" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="20"/>
+      <c r="B30" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C30" s="35" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" s="36"/>
+    </row>
+    <row r="31" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A31" s="20"/>
       <c r="B31" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C31" s="35" t="s">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="D31" s="36"/>
     </row>
     <row r="32" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A32" s="20"/>
       <c r="B32" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C32" s="35" t="s">
         <v>16</v>
@@ -1371,17 +1342,17 @@
     <row r="33" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A33" s="20"/>
       <c r="B33" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C33" s="35" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="36"/>
     </row>
-    <row r="34" spans="1:4" s="21" customFormat="1" ht="15" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A34" s="20"/>
       <c r="B34" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C34" s="35" t="s">
         <v>18</v>
@@ -1391,89 +1362,89 @@
     <row r="35" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A35" s="20"/>
       <c r="B35" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C35" s="35" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="D35" s="36"/>
     </row>
     <row r="36" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A36" s="20"/>
       <c r="B36" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C36" s="35" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="D36" s="36"/>
     </row>
-    <row r="37" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="20"/>
-      <c r="B37" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C37" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="D37" s="36"/>
-    </row>
-    <row r="38" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="20"/>
-      <c r="B38" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C38" s="35" t="s">
-        <v>22</v>
-      </c>
-      <c r="D38" s="36"/>
-    </row>
-    <row r="39" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="12"/>
+      <c r="B37" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C37" s="48"/>
+      <c r="D37" s="18">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A38" s="28">
+        <v>4</v>
+      </c>
+      <c r="B38" s="43" t="s">
+        <v>31</v>
+      </c>
+      <c r="C38" s="43"/>
+      <c r="D38" s="29">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" s="21" customFormat="1" ht="14.45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A39" s="20"/>
       <c r="B39" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C39" s="35" t="s">
-        <v>32</v>
+        <v>6</v>
       </c>
       <c r="D39" s="36"/>
     </row>
     <row r="40" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A40" s="20"/>
       <c r="B40" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C40" s="35" t="s">
-        <v>33</v>
+        <v>7</v>
       </c>
       <c r="D40" s="36"/>
     </row>
-    <row r="41" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="12"/>
-      <c r="B41" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C41" s="48"/>
-      <c r="D41" s="18">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A42" s="28">
-        <v>4</v>
-      </c>
-      <c r="B42" s="50" t="s">
-        <v>35</v>
-      </c>
-      <c r="C42" s="50"/>
-      <c r="D42" s="29">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" s="21" customFormat="1" ht="14.45" customHeight="1" outlineLevel="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" s="21" customFormat="1" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="20"/>
+      <c r="B41" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C41" s="35" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="36"/>
+    </row>
+    <row r="42" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="20"/>
+      <c r="B42" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C42" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42" s="36"/>
+    </row>
+    <row r="43" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A43" s="20"/>
       <c r="B43" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C43" s="35" t="s">
         <v>10</v>
@@ -1483,181 +1454,181 @@
     <row r="44" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A44" s="20"/>
       <c r="B44" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C44" s="35" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="36"/>
     </row>
-    <row r="45" spans="1:4" s="21" customFormat="1" ht="45" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="20"/>
-      <c r="B45" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C45" s="35" t="s">
-        <v>12</v>
-      </c>
-      <c r="D45" s="36"/>
-    </row>
-    <row r="46" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="20"/>
-      <c r="B46" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C46" s="35" t="s">
-        <v>13</v>
-      </c>
-      <c r="D46" s="36"/>
+    <row r="45" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="12"/>
+      <c r="B45" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="48"/>
+      <c r="D45" s="18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A46" s="28">
+        <v>5</v>
+      </c>
+      <c r="B46" s="43" t="s">
+        <v>45</v>
+      </c>
+      <c r="C46" s="43"/>
+      <c r="D46" s="29">
+        <v>60</v>
+      </c>
     </row>
     <row r="47" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A47" s="20"/>
       <c r="B47" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C47" s="35" t="s">
-        <v>14</v>
+        <v>49</v>
       </c>
       <c r="D47" s="36"/>
     </row>
     <row r="48" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A48" s="20"/>
       <c r="B48" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C48" s="35" t="s">
-        <v>15</v>
+        <v>48</v>
       </c>
       <c r="D48" s="36"/>
     </row>
-    <row r="49" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="12"/>
-      <c r="B49" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C49" s="48"/>
-      <c r="D49" s="18">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A50" s="28">
-        <v>5</v>
-      </c>
-      <c r="B50" s="50" t="s">
-        <v>49</v>
-      </c>
-      <c r="C50" s="50"/>
-      <c r="D50" s="29">
-        <v>60</v>
-      </c>
+    <row r="49" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="20"/>
+      <c r="B49" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C49" s="35" t="s">
+        <v>47</v>
+      </c>
+      <c r="D49" s="36"/>
+    </row>
+    <row r="50" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="20"/>
+      <c r="B50" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="D50" s="36"/>
     </row>
     <row r="51" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A51" s="20"/>
       <c r="B51" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C51" s="35" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D51" s="36"/>
     </row>
-    <row r="52" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="20"/>
+    <row r="52" spans="1:4" s="42" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="40"/>
       <c r="B52" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C52" s="35" t="s">
         <v>52</v>
       </c>
-      <c r="D52" s="36"/>
+      <c r="D52" s="41"/>
     </row>
     <row r="53" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A53" s="20"/>
       <c r="B53" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C53" s="35" t="s">
+        <v>67</v>
+      </c>
+      <c r="D53" s="36"/>
+    </row>
+    <row r="54" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="12"/>
+      <c r="B54" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C54" s="48"/>
+      <c r="D54" s="18">
         <v>30</v>
       </c>
-      <c r="C53" s="35" t="s">
-        <v>51</v>
-      </c>
-      <c r="D53" s="36"/>
-    </row>
-    <row r="54" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="20"/>
-      <c r="B54" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C54" s="21" t="s">
-        <v>54</v>
-      </c>
-      <c r="D54" s="36"/>
-    </row>
-    <row r="55" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="20"/>
-      <c r="B55" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C55" s="35" t="s">
-        <v>55</v>
-      </c>
-      <c r="D55" s="36"/>
-    </row>
-    <row r="56" spans="1:4" s="43" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="41"/>
+    </row>
+    <row r="55" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A55" s="28">
+        <v>6</v>
+      </c>
+      <c r="B55" s="43" t="s">
+        <v>53</v>
+      </c>
+      <c r="C55" s="43"/>
+      <c r="D55" s="29">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="20"/>
       <c r="B56" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C56" s="35" t="s">
-        <v>56</v>
-      </c>
-      <c r="D56" s="42"/>
+        <v>60</v>
+      </c>
+      <c r="D56" s="36"/>
     </row>
     <row r="57" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A57" s="20"/>
       <c r="B57" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C57" s="35" t="s">
-        <v>72</v>
+        <v>54</v>
       </c>
       <c r="D57" s="36"/>
     </row>
-    <row r="58" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="12"/>
-      <c r="B58" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C58" s="48"/>
-      <c r="D58" s="18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A59" s="28">
-        <v>6</v>
-      </c>
-      <c r="B59" s="50" t="s">
-        <v>57</v>
-      </c>
-      <c r="C59" s="50"/>
-      <c r="D59" s="29">
-        <v>75</v>
-      </c>
+    <row r="58" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="20"/>
+      <c r="B58" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C58" s="35" t="s">
+        <v>55</v>
+      </c>
+      <c r="D58" s="36"/>
+    </row>
+    <row r="59" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="20"/>
+      <c r="B59" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C59" s="35" t="s">
+        <v>56</v>
+      </c>
+      <c r="D59" s="36"/>
     </row>
     <row r="60" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A60" s="20"/>
       <c r="B60" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C60" s="35" t="s">
-        <v>64</v>
+        <v>57</v>
       </c>
       <c r="D60" s="36"/>
     </row>
     <row r="61" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A61" s="20"/>
       <c r="B61" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C61" s="35" t="s">
         <v>58</v>
@@ -1667,192 +1638,142 @@
     <row r="62" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A62" s="20"/>
       <c r="B62" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C62" s="35" t="s">
         <v>59</v>
       </c>
       <c r="D62" s="36"/>
     </row>
-    <row r="63" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="20"/>
-      <c r="B63" s="19" t="s">
+    <row r="63" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="12"/>
+      <c r="B63" s="48" t="s">
+        <v>25</v>
+      </c>
+      <c r="C63" s="48"/>
+      <c r="D63" s="18">
         <v>30</v>
       </c>
-      <c r="C63" s="35" t="s">
-        <v>60</v>
-      </c>
-      <c r="D63" s="36"/>
-    </row>
-    <row r="64" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="20"/>
-      <c r="B64" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C64" s="35" t="s">
-        <v>61</v>
-      </c>
-      <c r="D64" s="36"/>
+    </row>
+    <row r="64" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A64" s="28">
+        <v>7</v>
+      </c>
+      <c r="B64" s="43" t="s">
+        <v>62</v>
+      </c>
+      <c r="C64" s="43"/>
+      <c r="D64" s="29">
+        <v>90</v>
+      </c>
     </row>
     <row r="65" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A65" s="20"/>
       <c r="B65" s="19" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="C65" s="35" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D65" s="36"/>
     </row>
     <row r="66" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
       <c r="A66" s="20"/>
       <c r="B66" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C66" s="39" t="s">
+        <v>64</v>
+      </c>
+      <c r="D66" s="36"/>
+    </row>
+    <row r="67" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="20"/>
+      <c r="B67" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C67" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="D67" s="36"/>
+    </row>
+    <row r="68" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="20"/>
+      <c r="B68" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="C68" s="35" t="s">
+        <v>66</v>
+      </c>
+      <c r="D68" s="36"/>
+    </row>
+    <row r="69" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="31"/>
+      <c r="B69" s="49" t="s">
+        <v>25</v>
+      </c>
+      <c r="C69" s="49"/>
+      <c r="D69" s="32">
         <v>30</v>
       </c>
-      <c r="C66" s="35" t="s">
-        <v>63</v>
-      </c>
-      <c r="D66" s="36"/>
-    </row>
-    <row r="67" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="12"/>
-      <c r="B67" s="48" t="s">
-        <v>29</v>
-      </c>
-      <c r="C67" s="48"/>
-      <c r="D67" s="18">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" s="11" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A68" s="28">
-        <v>7</v>
-      </c>
-      <c r="B68" s="50" t="s">
-        <v>66</v>
-      </c>
-      <c r="C68" s="50"/>
-      <c r="D68" s="29">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="20"/>
-      <c r="B69" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C69" s="35" t="s">
-        <v>67</v>
-      </c>
-      <c r="D69" s="36"/>
-    </row>
-    <row r="70" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A70" s="20"/>
-      <c r="B70" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C70" s="39" t="s">
-        <v>69</v>
-      </c>
-      <c r="D70" s="36"/>
-    </row>
-    <row r="71" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A71" s="20"/>
-      <c r="B71" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C71" s="40" t="s">
-        <v>68</v>
-      </c>
-      <c r="D71" s="36"/>
-    </row>
-    <row r="72" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="20"/>
-      <c r="B72" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C72" s="21" t="s">
-        <v>70</v>
-      </c>
-      <c r="D72" s="36"/>
-    </row>
-    <row r="73" spans="1:4" s="21" customFormat="1" outlineLevel="1" x14ac:dyDescent="0.25">
-      <c r="A73" s="20"/>
-      <c r="B73" s="19" t="s">
-        <v>30</v>
-      </c>
-      <c r="C73" s="35" t="s">
-        <v>71</v>
-      </c>
-      <c r="D73" s="36"/>
-    </row>
-    <row r="74" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A74" s="31"/>
-      <c r="B74" s="49" t="s">
-        <v>29</v>
-      </c>
-      <c r="C74" s="49"/>
-      <c r="D74" s="32">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A75" s="15" t="s">
-        <v>23</v>
-      </c>
-      <c r="B75" s="51" t="s">
-        <v>25</v>
-      </c>
-      <c r="C75" s="51"/>
-      <c r="D75" s="30">
-        <f>SUM(D4:D74)</f>
+    </row>
+    <row r="70" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A70" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B70" s="50" t="s">
+        <v>21</v>
+      </c>
+      <c r="C70" s="50"/>
+      <c r="D70" s="30">
+        <f>SUM(D4:D69)</f>
         <v>800</v>
       </c>
     </row>
-    <row r="76" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="33" t="s">
-        <v>23</v>
-      </c>
-      <c r="B76" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="C76" s="47"/>
-      <c r="D76" s="34">
-        <f>ROUND(D75/60,1)</f>
+    <row r="71" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A71" s="33" t="s">
+        <v>19</v>
+      </c>
+      <c r="B71" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C71" s="47"/>
+      <c r="D71" s="34">
+        <f>ROUND(D70/60,1)</f>
         <v>13.3</v>
       </c>
     </row>
-    <row r="77" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="7"/>
-      <c r="B77" s="7"/>
-      <c r="C77" s="8"/>
-      <c r="D77" s="9"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="4"/>
-      <c r="B78" s="4"/>
-      <c r="C78" s="5"/>
-      <c r="D78" s="6"/>
+    <row r="72" spans="1:4" s="10" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="7"/>
+      <c r="B72" s="7"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="9"/>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="4"/>
+      <c r="B73" s="4"/>
+      <c r="C73" s="5"/>
+      <c r="D73" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B71:C71"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B45:C45"/>
+    <mergeCell ref="B54:C54"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B69:C69"/>
+    <mergeCell ref="B46:C46"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="B70:C70"/>
+    <mergeCell ref="B38:C38"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B5:C5"/>
     <mergeCell ref="B6:C6"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B49:C49"/>
-    <mergeCell ref="B58:C58"/>
-    <mergeCell ref="B67:C67"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B74:C74"/>
-    <mergeCell ref="B50:C50"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B68:C68"/>
-    <mergeCell ref="B75:C75"/>
+    <mergeCell ref="B16:C16"/>
   </mergeCells>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup paperSize="9" scale="91" fitToHeight="0" orientation="portrait" r:id="rId1"/>

</xml_diff>